<commit_message>
saturday before monday meeting with finca - before filter
</commit_message>
<xml_diff>
--- a/ErroresImportacionExcel.xlsx
+++ b/ErroresImportacionExcel.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -39,12 +39,18 @@
       <color rgb="ffffff"/>
     </font>
     <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <b/>
+      <color rgb="ffffff"/>
+    </font>
+    <font>
       <sz val="14"/>
       <name val="Calibri"/>
       <color rgb="000000"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none">
         <bgColor/>
@@ -69,7 +75,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7395bb"/>
+        <fgColor rgb="FFe3f2fd"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFe3f2fd"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -93,7 +105,7 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -106,7 +118,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,14 +455,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="64.28125" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="64.28125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -462,13 +477,24 @@
       <c r="B2" s="5" t="str">
         <v>Errores de inserción</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="6" t="str">
         <v>Descripción</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="str">
-        <v>4</v>
+      <c r="A3" s="7" t="str">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="str">
+        <v>Activo: Cuenta</v>
+      </c>
+      <c r="C3" s="7" t="str">
+        <v>No existe un monto FOSEDE para el tipo de moneda</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="str">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>